<commit_message>
Added Rev5 Fabrication Files
</commit_message>
<xml_diff>
--- a/PCB/production/BOM with D2.xlsx
+++ b/PCB/production/BOM with D2.xlsx
@@ -1,52 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\Omote Updated JLC Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A933FB2-CC42-4C89-BD3F-AE54AAF48F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC38767-9CF5-47D3-8270-24C86C662C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="915" windowWidth="18210" windowHeight="13890" xr2:uid="{0D1F3E65-C25E-4AA9-A4C8-FF6E85BADB4A}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM JLC" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
   <si>
     <t>Designator</t>
   </si>
   <si>
+    <t>Footprint</t>
+  </si>
+  <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>LCSC Part #</t>
   </si>
   <si>
-    <t>AE1</t>
-  </si>
-  <si>
-    <t>Antenna</t>
-  </si>
-  <si>
-    <t>RFANT5220110A2T</t>
-  </si>
-  <si>
-    <t>C454142</t>
-  </si>
-  <si>
-    <t>C1, C10, C12, C14, C17, C20, C22, C23, C24, C26, C9</t>
+    <t>C1, C10, C12, C17, C20, C22, C23, C24, C26, C29, C9</t>
   </si>
   <si>
     <t>100nF</t>
@@ -55,16 +48,7 @@
     <t>C1591</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>C913904</t>
-  </si>
-  <si>
-    <t>C13, C16, C21, C25, C28, C3, C5, C6, C7, C8</t>
+    <t>C11, C13, C14, C16, C18, C21, C25, C28, C3, C5, C6, C7, C8</t>
   </si>
   <si>
     <t>10uF</t>
@@ -85,16 +69,16 @@
     <t>D1</t>
   </si>
   <si>
-    <t>MBR0520</t>
-  </si>
-  <si>
-    <t>D_SOD-123</t>
-  </si>
-  <si>
-    <t>C475717</t>
-  </si>
-  <si>
-    <t>D3, D4, D5</t>
+    <t>D_SOD-323</t>
+  </si>
+  <si>
+    <t>BAT20J</t>
+  </si>
+  <si>
+    <t>C155590</t>
+  </si>
+  <si>
+    <t>D10, D11, D12, D13, D14, D15, D16, D3, D4, D5, D6, D7, D8, D9</t>
   </si>
   <si>
     <t>LED</t>
@@ -115,76 +99,88 @@
     <t>J1</t>
   </si>
   <si>
+    <t>USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
+  </si>
+  <si>
     <t>USB_C_Receptacle_USB2.0</t>
   </si>
   <si>
-    <t>USB_C_Receptacle_HRO_TYPE-C-31-M-12</t>
-  </si>
-  <si>
     <t>C2982555</t>
   </si>
   <si>
     <t>J2</t>
   </si>
   <si>
+    <t>TFT_2.83IN_240X320_50PIN</t>
+  </si>
+  <si>
     <t>Conn_01x50</t>
   </si>
   <si>
-    <t>TFT_2.83IN_240X320_50PIN</t>
-  </si>
-  <si>
     <t>C11098</t>
   </si>
   <si>
     <t>J3</t>
   </si>
   <si>
+    <t>JST_PH_B2B-PH-SM4-TB_1x02-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
     <t>JST_PH_B2B-PH</t>
   </si>
   <si>
-    <t>JST_PH_B2B-PH-SM4-TB_1x02-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
     <t>C160352</t>
   </si>
   <si>
-    <t>Q1, Q3, Q4, Q5</t>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>MicroSD Slot TF-01A</t>
+  </si>
+  <si>
+    <t>Micro_SD_Card</t>
+  </si>
+  <si>
+    <t>C20613191</t>
+  </si>
+  <si>
+    <t>Q1, Q3, Q4, Q5, Q7</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
   </si>
   <si>
     <t>DMG2301L</t>
   </si>
   <si>
-    <t>SOT-23</t>
-  </si>
-  <si>
     <t>C102619</t>
   </si>
   <si>
     <t>Q2</t>
   </si>
   <si>
+    <t>SOT-363_SC-70-6</t>
+  </si>
+  <si>
     <t>MBT3904DW1</t>
   </si>
   <si>
-    <t>SOT-363_SC-70-6</t>
-  </si>
-  <si>
     <t>C110150</t>
   </si>
   <si>
     <t>Q6</t>
   </si>
   <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
     <t>FS8205A</t>
   </si>
   <si>
-    <t>SOT-23-6</t>
-  </si>
-  <si>
     <t>C908265</t>
   </si>
   <si>
-    <t>R1, R39, R40, R5</t>
+    <t>R1, R23, R31, R32, R33, R34, R35, R38, R39, R40, R41, R42, R43, R44, R5</t>
   </si>
   <si>
     <t>2k2</t>
@@ -193,6 +189,15 @@
     <t>C114662</t>
   </si>
   <si>
+    <t>R10, R13, R14, R19, R20, R22, R24, R26, R30, R36, R37, R6</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>C98220</t>
+  </si>
+  <si>
     <t>R11, R12, R25, R8</t>
   </si>
   <si>
@@ -202,21 +207,18 @@
     <t>C99782</t>
   </si>
   <si>
-    <t>R13, R14, R19, R20, R22, R23, R26, R30, R31, R32, R33, R34, R35, R37, R6</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>C98220</t>
-  </si>
-  <si>
     <t>R15, R16, R17, R18</t>
   </si>
   <si>
     <t>C109318</t>
   </si>
   <si>
+    <t>R2, R27, R28, R29</t>
+  </si>
+  <si>
+    <t>C105881</t>
+  </si>
+  <si>
     <t>R21</t>
   </si>
   <si>
@@ -226,12 +228,6 @@
     <t>C2849062</t>
   </si>
   <si>
-    <t>R27, R28, R29</t>
-  </si>
-  <si>
-    <t>C105881</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -241,12 +237,6 @@
     <t>C22548</t>
   </si>
   <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t>C116699</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -259,18 +249,18 @@
     <t>5.1k</t>
   </si>
   <si>
-    <t>C105580</t>
+    <t>C114626</t>
   </si>
   <si>
     <t>S1, S10, S11, S12, S13, S14, S15, S16, S17, S18, S19, S2, S20, S22, S23, S24, S25, S26, S3, S4, S5, S6, S7, S8, S9</t>
   </si>
   <si>
+    <t>SW_SPST_TL3342</t>
+  </si>
+  <si>
     <t>TL3342F160QG</t>
   </si>
   <si>
-    <t>SW_SPST_TL3342</t>
-  </si>
-  <si>
     <t xml:space="preserve">C778172 </t>
   </si>
   <si>
@@ -286,85 +276,97 @@
     <t>U11</t>
   </si>
   <si>
+    <t>Infineon_PG-DSO-8-27_3.9x4.9mm_EP2.65x3mm</t>
+  </si>
+  <si>
     <t>TP4056</t>
   </si>
   <si>
-    <t>Infineon_PG-DSO-8-27_3.9x4.9mm_EP2.65x3mm</t>
-  </si>
-  <si>
     <t>C725790</t>
   </si>
   <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>HVQFN-24-1EP_4x4mm_P0.5mm_EP2.5x2.5mm</t>
+  </si>
+  <si>
+    <t>TCA8418</t>
+  </si>
+  <si>
+    <t>C138713</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
     <t>XC6220B331</t>
   </si>
   <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
     <t>C86534</t>
   </si>
   <si>
     <t>U3</t>
   </si>
   <si>
+    <t>SOIC-16_3.9x9.9mm_P1.27mm</t>
+  </si>
+  <si>
     <t>CH340C</t>
   </si>
   <si>
-    <t>SOIC-16_3.9x9.9mm_P1.27mm</t>
-  </si>
-  <si>
     <t>C84681</t>
   </si>
   <si>
     <t>U4</t>
   </si>
   <si>
+    <t>SOT-666</t>
+  </si>
+  <si>
     <t>USBLC6-2P6</t>
   </si>
   <si>
-    <t>SOT-666</t>
-  </si>
-  <si>
     <t>C2827693</t>
   </si>
   <si>
     <t>U5</t>
   </si>
   <si>
+    <t>XDCR_LIS3DHTR</t>
+  </si>
+  <si>
     <t>LIS3DHTR</t>
   </si>
   <si>
-    <t>XDCR_LIS3DHTR</t>
-  </si>
-  <si>
     <t>C15134</t>
   </si>
   <si>
     <t>U6</t>
   </si>
   <si>
+    <t>Heimdall vertical</t>
+  </si>
+  <si>
     <t>TSSP77038</t>
   </si>
   <si>
-    <t>Heimdall vertical</t>
-  </si>
-  <si>
-    <t>C499566</t>
+    <t>C3291489</t>
   </si>
   <si>
     <t>U7</t>
   </si>
   <si>
-    <t>ESP32-PICO-D4</t>
-  </si>
-  <si>
-    <t>QFN-48-1EP_7x7mm_P0.5mm_EP5.3x5.3mm_ThermalVias_MR</t>
-  </si>
-  <si>
-    <t>C193707</t>
+    <t>ESP32-S3-WROOM-1</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1-N16R8</t>
+  </si>
+  <si>
+    <t>C2913202</t>
   </si>
   <si>
     <t>U8</t>
@@ -379,10 +381,10 @@
     <t>U9</t>
   </si>
   <si>
+    <t>TDFN-8-1EP_2x2mm_P0.5mm_EP0.8x1.2mm</t>
+  </si>
+  <si>
     <t>MAX17048G</t>
-  </si>
-  <si>
-    <t>TDFN-8-1EP_2x2mm_P0.5mm_EP0.8x1.2mm</t>
   </si>
   <si>
     <t>C2682616</t>
@@ -410,40 +412,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -451,283 +423,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -735,204 +445,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1243,32 +765,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1E7009-FF7F-4F01-8053-7357149DCFC6}">
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="93.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1279,50 +800,50 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>603</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>805</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3">
-        <v>603</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4">
         <v>603</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>805</v>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -1344,41 +865,41 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" t="s">
-        <v>126</v>
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>1206</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9">
-        <v>603</v>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -1389,94 +910,94 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10">
-        <v>1206</v>
-      </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" t="s">
         <v>52</v>
+      </c>
+      <c r="C16">
+        <v>603</v>
       </c>
       <c r="D16" t="s">
         <v>53</v>
@@ -1514,50 +1035,50 @@
       <c r="A19" t="s">
         <v>60</v>
       </c>
-      <c r="B19" t="s">
-        <v>61</v>
+      <c r="B19">
+        <v>10</v>
       </c>
       <c r="C19">
         <v>603</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>330</v>
       </c>
       <c r="C20">
         <v>603</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
         <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>66</v>
       </c>
       <c r="C21">
         <v>805</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
         <v>68</v>
-      </c>
-      <c r="B22">
-        <v>330</v>
       </c>
       <c r="C22">
         <v>603</v>
@@ -1570,22 +1091,22 @@
       <c r="A23" t="s">
         <v>70</v>
       </c>
-      <c r="B23" t="s">
-        <v>71</v>
+      <c r="B23">
+        <v>100</v>
       </c>
       <c r="C23">
         <v>603</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
         <v>73</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
       </c>
       <c r="C24">
         <v>603</v>
@@ -1598,181 +1119,172 @@
       <c r="A25" t="s">
         <v>75</v>
       </c>
-      <c r="B25">
-        <v>100</v>
-      </c>
-      <c r="C25">
-        <v>603</v>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26">
-        <v>603</v>
+        <v>80</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" t="s">
         <v>120</v>
       </c>
-      <c r="D37" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1781,12 +1293,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>123</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed LCSC number for R7/R9
The LCSC part number  for R7 and R9 was wrongly linked to a 5.1 Ohm resistor instead of a 5.1 KiloOhm resistor.
</commit_message>
<xml_diff>
--- a/PCB/production/BOM with D2.xlsx
+++ b/PCB/production/BOM with D2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Documents\GitHub\OMOTE\PCB\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC38767-9CF5-47D3-8270-24C86C662C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6FD8D6-4C0C-4E07-A0B3-390A47BAC414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="915" windowWidth="18210" windowHeight="13890" xr2:uid="{0D1F3E65-C25E-4AA9-A4C8-FF6E85BADB4A}"/>
+    <workbookView xWindow="18990" yWindow="1065" windowWidth="18210" windowHeight="13890" xr2:uid="{0D1F3E65-C25E-4AA9-A4C8-FF6E85BADB4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -249,9 +249,6 @@
     <t>5.1k</t>
   </si>
   <si>
-    <t>C114626</t>
-  </si>
-  <si>
     <t>S1, S10, S11, S12, S13, S14, S15, S16, S17, S18, S19, S2, S20, S22, S23, S24, S25, S26, S3, S4, S5, S6, S7, S8, S9</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>C405273</t>
+  </si>
+  <si>
+    <t>C105580</t>
   </si>
 </sst>
 </file>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F1E7009-FF7F-4F01-8053-7357149DCFC6}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,16 +865,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
         <v>123</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>124</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>125</v>
-      </c>
-      <c r="D7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,185 +1112,185 @@
         <v>603</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
         <v>79</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
         <v>82</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>84</v>
-      </c>
-      <c r="C27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" t="s">
         <v>86</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>88</v>
-      </c>
-      <c r="C28" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
         <v>90</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>92</v>
-      </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
         <v>94</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>96</v>
-      </c>
-      <c r="C30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
         <v>98</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>100</v>
-      </c>
-      <c r="C31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
         <v>102</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>104</v>
-      </c>
-      <c r="C32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" t="s">
         <v>106</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>108</v>
-      </c>
-      <c r="C33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" t="s">
         <v>110</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>112</v>
-      </c>
-      <c r="C34" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
         <v>114</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" t="s">
         <v>115</v>
-      </c>
-      <c r="C35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>119</v>
-      </c>
-      <c r="C36" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>